<commit_message>
instructions for FC and Prod
</commit_message>
<xml_diff>
--- a/Lists/Voi_FC.xlsx
+++ b/Lists/Voi_FC.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\ortexp\Lists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julianrl_adm\Experiment_Orthography\Lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="170">
   <si>
     <t>Trigger_txt</t>
   </si>
@@ -531,6 +531,9 @@
   </si>
   <si>
     <t>maluk</t>
+  </si>
+  <si>
+    <t>Instr</t>
   </si>
 </sst>
 </file>
@@ -586,7 +589,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -848,20 +851,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2:K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="31.28515625" customWidth="1"/>
-    <col min="7" max="7" width="35.5703125" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" customWidth="1"/>
+    <col min="7" max="7" width="35.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -892,8 +895,11 @@
       <c r="J1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -924,8 +930,12 @@
       <c r="J2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="str">
+        <f>IF(J2="pl","Choose the plural form of the word that belongs to the language","Choose the singular form of the word that belongs to the language")</f>
+        <v>Choose the plural form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -956,8 +966,12 @@
       <c r="J3" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K31" si="0">IF(J3="pl","Choose the plural form of the word that belongs to the language","Choose the singular form of the word that belongs to the language")</f>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -988,8 +1002,12 @@
       <c r="J4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the plural form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1020,8 +1038,12 @@
       <c r="J5" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -1052,8 +1074,12 @@
       <c r="J6" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1084,8 +1110,12 @@
       <c r="J7" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -1116,8 +1146,12 @@
       <c r="J8" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -1148,8 +1182,12 @@
       <c r="J9" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1180,8 +1218,12 @@
       <c r="J10" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the plural form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1212,8 +1254,12 @@
       <c r="J11" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1244,8 +1290,12 @@
       <c r="J12" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the plural form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1276,8 +1326,12 @@
       <c r="J13" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -1308,8 +1362,12 @@
       <c r="J14" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -1340,8 +1398,12 @@
       <c r="J15" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -1372,8 +1434,12 @@
       <c r="J16" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -1404,8 +1470,12 @@
       <c r="J17" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1436,8 +1506,12 @@
       <c r="J18" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the plural form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1468,8 +1542,12 @@
       <c r="J19" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1500,8 +1578,12 @@
       <c r="J20" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1532,8 +1614,12 @@
       <c r="J21" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -1564,8 +1650,12 @@
       <c r="J22" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -1596,8 +1686,12 @@
       <c r="J23" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>88</v>
       </c>
@@ -1628,8 +1722,12 @@
       <c r="J24" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>93</v>
       </c>
@@ -1660,8 +1758,12 @@
       <c r="J25" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the plural form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -1692,8 +1794,12 @@
       <c r="J26" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the plural form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>112</v>
       </c>
@@ -1724,8 +1830,12 @@
       <c r="J27" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -1756,8 +1866,12 @@
       <c r="J28" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -1788,8 +1902,12 @@
       <c r="J29" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>116</v>
       </c>
@@ -1820,8 +1938,12 @@
       <c r="J30" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the singular form of the word that belongs to the language</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>149</v>
       </c>
@@ -1851,6 +1973,10 @@
       </c>
       <c r="J31" t="s">
         <v>165</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="0"/>
+        <v>Choose the plural form of the word that belongs to the language</v>
       </c>
     </row>
   </sheetData>

</xml_diff>